<commit_message>
Updated Sprint 2 Backlog with new items
1) Updated progress and added new items
</commit_message>
<xml_diff>
--- a/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
+++ b/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BE24CA-CA75-4A98-AB33-126238B29969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CCC2EA-81A8-40DC-A847-9451F3146EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Related User Story</t>
   </si>
@@ -150,6 +150,27 @@
   </si>
   <si>
     <t>Jabesi</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Jabesi, Jacob</t>
+  </si>
+  <si>
+    <t>Testing &amp; Documentation</t>
+  </si>
+  <si>
+    <t>Test User Management</t>
+  </si>
+  <si>
+    <t>Test Group Management</t>
+  </si>
+  <si>
+    <t>Test remaining classes</t>
+  </si>
+  <si>
+    <t>Fix Class diagram</t>
   </si>
 </sst>
 </file>
@@ -184,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3A1FD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF88CDC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +350,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -334,6 +361,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF88CDC"/>
       <color rgb="FFD3A1FD"/>
     </mruColors>
   </colors>
@@ -440,12 +468,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$31:$H$31</c:f>
+              <c:f>Sheet1!$D$36:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1207,7 +1235,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1499,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1647,9 @@
       <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1631,10 +1661,18 @@
       <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
@@ -1643,10 +1681,18 @@
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
@@ -1670,9 +1716,15 @@
       <c r="C12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
@@ -1684,9 +1736,15 @@
       <c r="C13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="D13" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
@@ -1707,7 +1765,9 @@
       <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1719,7 +1779,9 @@
       <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D16" s="12"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -1731,7 +1793,9 @@
       <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="12"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1767,7 +1831,9 @@
       <c r="B20" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1779,7 +1845,9 @@
       <c r="B21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1788,10 +1856,12 @@
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -1861,60 +1931,124 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="22">
+        <v>8</v>
+      </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1">
-        <f>SUM(D3:D30)</f>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1">
+        <f>SUM(D3:D35)</f>
+        <v>13.5</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:H36" si="0">SUM(E3:E35)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="1">
-        <f t="shared" ref="E31:H31" si="0">SUM(E3:E30)</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="F36" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G36" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H36" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1934,12 +2068,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2083,6 +2211,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2093,15 +2227,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2119,6 +2244,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Changed actual work hours
</commit_message>
<xml_diff>
--- a/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
+++ b/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja00069\Downloads\CapstoneGroup3\sprints\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65154A-50D2-450F-9453-9A754751529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252CAE1D-75CA-4E4B-84EF-BF8D03F0CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Related User Story</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Fix Class diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Project Management </t>
+  </si>
+  <si>
+    <t>Add Group Aproval Process</t>
+  </si>
+  <si>
+    <t>Add Project List Filtering</t>
+  </si>
+  <si>
+    <t>Update Wireframe</t>
   </si>
 </sst>
 </file>
@@ -468,21 +480,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$36:$H$36</c:f>
+              <c:f>Sheet1!$D$39:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>29.5</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1235,7 +1247,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1527,16 +1539,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="151.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -1864,9 +1876,15 @@
       <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="D20" s="5">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9">
+        <v>4</v>
+      </c>
+      <c r="F20" s="9">
+        <v>7</v>
+      </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
@@ -1878,9 +1896,15 @@
       <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="D21" s="5">
+        <v>10</v>
+      </c>
+      <c r="E21" s="9">
+        <v>5</v>
+      </c>
+      <c r="F21" s="9">
+        <v>6</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
@@ -1892,9 +1916,15 @@
       <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9">
+        <v>5</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
@@ -1906,54 +1936,76 @@
       <c r="C23" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="D23" s="15">
+        <v>5</v>
+      </c>
+      <c r="E23" s="14">
+        <v>4</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0</v>
+      </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="B24" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="15">
+        <v>3</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
+      <c r="F24" s="14">
+        <v>3</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="15">
+        <v>4</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="17"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1962,8 +2014,10 @@
     </row>
     <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="18"/>
       <c r="D28" s="17"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1971,46 +2025,40 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="20">
-        <v>8</v>
-      </c>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="20">
-        <v>6</v>
-      </c>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
+      <c r="A31" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="B31" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+        <v>41</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="20">
+        <v>8</v>
+      </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -2019,10 +2067,14 @@
     <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="20">
+        <v>6</v>
+      </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -2030,7 +2082,9 @@
     </row>
     <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
+      <c r="B33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="9"/>
@@ -2039,50 +2093,110 @@
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="9"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="20">
+        <v>6</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
       <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="G34" s="9">
+        <v>6</v>
+      </c>
       <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="19" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="20">
+        <v>2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="20">
         <v>9</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9">
+        <v>11</v>
+      </c>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1">
-        <f>SUM(D3:D35)</f>
-        <v>29.5</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" ref="E36:H36" si="0">SUM(E3:E35)</f>
-        <v>5</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1">
+        <f>SUM(D3:D38)</f>
+        <v>83.5</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" ref="E39:H39" si="0">SUM(E3:E38)</f>
+        <v>23</v>
+      </c>
+      <c r="F39" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G36" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="G39" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
+        <v>18</v>
+      </c>
+      <c r="H39" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2102,12 +2216,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2251,6 +2359,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2261,15 +2375,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2287,6 +2392,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update Sprint 2 Backlog Burndown
</commit_message>
<xml_diff>
--- a/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
+++ b/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja00069\Downloads\CapstoneGroup3\sprints\sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252CAE1D-75CA-4E4B-84EF-BF8D03F0CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D723879-45C1-4926-BCE8-3B4D6800895E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Related User Story</t>
   </si>
@@ -485,13 +485,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>83.5</c:v>
+                  <c:v>86.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18</c:v>
@@ -1541,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1819,7 +1819,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1849,10 +1849,18 @@
       <c r="B18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="C18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="12">
+        <v>3</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -2182,7 +2190,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1">
         <f>SUM(D3:D38)</f>
-        <v>83.5</v>
+        <v>86.5</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" ref="E39:H39" si="0">SUM(E3:E38)</f>
@@ -2190,7 +2198,7 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>35</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="0"/>
@@ -2216,6 +2224,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2359,12 +2373,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2375,6 +2383,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2392,15 +2409,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>